<commit_message>
Iniciamos nuevamente el proyecto
</commit_message>
<xml_diff>
--- a/Diagrama Gantt Proyecto.xlsx
+++ b/Diagrama Gantt Proyecto.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{721E80F0-7AD0-47FB-B996-B0266BC04541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C9917B-0511-440B-A713-95D02FEE78DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="62">
   <si>
     <t>Crea una programación para un proyecto en esta hoja de cálculo.
 Escribe el título de este proyecto en la celda B1. 
@@ -250,6 +250,21 @@
   </si>
   <si>
     <t>Willy Corzo</t>
+  </si>
+  <si>
+    <t>Arquitectura Limpia</t>
+  </si>
+  <si>
+    <t>Manejo de estados</t>
+  </si>
+  <si>
+    <t>Modulo de Almacenamiento Local</t>
+  </si>
+  <si>
+    <t>Peticiones Get</t>
+  </si>
+  <si>
+    <t>Implementacion Locacion Geografica</t>
   </si>
 </sst>
 </file>
@@ -1290,6 +1305,13 @@
     <xf numFmtId="172" fontId="9" fillId="10" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="170" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1302,13 +1324,6 @@
     <xf numFmtId="169" fontId="9" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="54">
     <cellStyle name="20% - Énfasis1" xfId="31" builtinId="30" customBuiltin="1"/>
@@ -1919,8 +1934,8 @@
   <dimension ref="A1:BL41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <pane ySplit="6" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1971,117 +1986,117 @@
       <c r="B3" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="89" t="s">
+      <c r="C3" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="90"/>
-      <c r="E3" s="88">
+      <c r="D3" s="86"/>
+      <c r="E3" s="91">
         <v>44515</v>
       </c>
-      <c r="F3" s="88"/>
+      <c r="F3" s="91"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="89" t="s">
+      <c r="C4" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="90"/>
+      <c r="D4" s="86"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="85">
+      <c r="I4" s="88">
         <f>I5</f>
         <v>44515</v>
       </c>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
-      <c r="L4" s="86"/>
-      <c r="M4" s="86"/>
-      <c r="N4" s="86"/>
-      <c r="O4" s="87"/>
-      <c r="P4" s="85">
+      <c r="J4" s="89"/>
+      <c r="K4" s="89"/>
+      <c r="L4" s="89"/>
+      <c r="M4" s="89"/>
+      <c r="N4" s="89"/>
+      <c r="O4" s="90"/>
+      <c r="P4" s="88">
         <f>P5</f>
         <v>44522</v>
       </c>
-      <c r="Q4" s="86"/>
-      <c r="R4" s="86"/>
-      <c r="S4" s="86"/>
-      <c r="T4" s="86"/>
-      <c r="U4" s="86"/>
-      <c r="V4" s="87"/>
-      <c r="W4" s="85">
+      <c r="Q4" s="89"/>
+      <c r="R4" s="89"/>
+      <c r="S4" s="89"/>
+      <c r="T4" s="89"/>
+      <c r="U4" s="89"/>
+      <c r="V4" s="90"/>
+      <c r="W4" s="88">
         <f>W5</f>
         <v>44529</v>
       </c>
-      <c r="X4" s="86"/>
-      <c r="Y4" s="86"/>
-      <c r="Z4" s="86"/>
-      <c r="AA4" s="86"/>
-      <c r="AB4" s="86"/>
-      <c r="AC4" s="87"/>
-      <c r="AD4" s="85">
+      <c r="X4" s="89"/>
+      <c r="Y4" s="89"/>
+      <c r="Z4" s="89"/>
+      <c r="AA4" s="89"/>
+      <c r="AB4" s="89"/>
+      <c r="AC4" s="90"/>
+      <c r="AD4" s="88">
         <f>AD5</f>
         <v>44536</v>
       </c>
-      <c r="AE4" s="86"/>
-      <c r="AF4" s="86"/>
-      <c r="AG4" s="86"/>
-      <c r="AH4" s="86"/>
-      <c r="AI4" s="86"/>
-      <c r="AJ4" s="87"/>
-      <c r="AK4" s="85">
+      <c r="AE4" s="89"/>
+      <c r="AF4" s="89"/>
+      <c r="AG4" s="89"/>
+      <c r="AH4" s="89"/>
+      <c r="AI4" s="89"/>
+      <c r="AJ4" s="90"/>
+      <c r="AK4" s="88">
         <f>AK5</f>
         <v>44543</v>
       </c>
-      <c r="AL4" s="86"/>
-      <c r="AM4" s="86"/>
-      <c r="AN4" s="86"/>
-      <c r="AO4" s="86"/>
-      <c r="AP4" s="86"/>
-      <c r="AQ4" s="87"/>
-      <c r="AR4" s="85">
+      <c r="AL4" s="89"/>
+      <c r="AM4" s="89"/>
+      <c r="AN4" s="89"/>
+      <c r="AO4" s="89"/>
+      <c r="AP4" s="89"/>
+      <c r="AQ4" s="90"/>
+      <c r="AR4" s="88">
         <f>AR5</f>
         <v>44550</v>
       </c>
-      <c r="AS4" s="86"/>
-      <c r="AT4" s="86"/>
-      <c r="AU4" s="86"/>
-      <c r="AV4" s="86"/>
-      <c r="AW4" s="86"/>
-      <c r="AX4" s="87"/>
-      <c r="AY4" s="85">
+      <c r="AS4" s="89"/>
+      <c r="AT4" s="89"/>
+      <c r="AU4" s="89"/>
+      <c r="AV4" s="89"/>
+      <c r="AW4" s="89"/>
+      <c r="AX4" s="90"/>
+      <c r="AY4" s="88">
         <f>AY5</f>
         <v>44557</v>
       </c>
-      <c r="AZ4" s="86"/>
-      <c r="BA4" s="86"/>
-      <c r="BB4" s="86"/>
-      <c r="BC4" s="86"/>
-      <c r="BD4" s="86"/>
-      <c r="BE4" s="87"/>
-      <c r="BF4" s="85">
+      <c r="AZ4" s="89"/>
+      <c r="BA4" s="89"/>
+      <c r="BB4" s="89"/>
+      <c r="BC4" s="89"/>
+      <c r="BD4" s="89"/>
+      <c r="BE4" s="90"/>
+      <c r="BF4" s="88">
         <f>BF5</f>
         <v>44564</v>
       </c>
-      <c r="BG4" s="86"/>
-      <c r="BH4" s="86"/>
-      <c r="BI4" s="86"/>
-      <c r="BJ4" s="86"/>
-      <c r="BK4" s="86"/>
-      <c r="BL4" s="87"/>
+      <c r="BG4" s="89"/>
+      <c r="BH4" s="89"/>
+      <c r="BI4" s="89"/>
+      <c r="BJ4" s="89"/>
+      <c r="BK4" s="89"/>
+      <c r="BL4" s="90"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="91"/>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
       <c r="I5" s="78">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>44515</v>
@@ -3097,7 +3112,7 @@
     <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="46"/>
       <c r="B14" s="63" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="C14" s="56"/>
       <c r="D14" s="20">
@@ -3176,7 +3191,7 @@
     <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="45"/>
       <c r="B15" s="63" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="C15" s="56"/>
       <c r="D15" s="20">
@@ -3187,13 +3202,13 @@
         <v>44527</v>
       </c>
       <c r="F15" s="82">
-        <f>E15+5</f>
-        <v>44532</v>
+        <f>E15+4</f>
+        <v>44531</v>
       </c>
       <c r="G15" s="14"/>
       <c r="H15" s="14">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I15" s="31"/>
       <c r="J15" s="31"/>
@@ -3261,16 +3276,16 @@
       <c r="D16" s="20"/>
       <c r="E16" s="82">
         <f>F15</f>
-        <v>44532</v>
+        <v>44531</v>
       </c>
       <c r="F16" s="82">
-        <f>E16+3</f>
-        <v>44535</v>
+        <f>E16+0</f>
+        <v>44531</v>
       </c>
       <c r="G16" s="14"/>
       <c r="H16" s="14">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I16" s="31"/>
       <c r="J16" s="31"/>
@@ -3338,16 +3353,16 @@
       <c r="D17" s="20"/>
       <c r="E17" s="82">
         <f>E16</f>
-        <v>44532</v>
+        <v>44531</v>
       </c>
       <c r="F17" s="82">
-        <f>E17+2</f>
-        <v>44534</v>
+        <f>E17+0</f>
+        <v>44531</v>
       </c>
       <c r="G17" s="14"/>
       <c r="H17" s="14">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I17" s="31"/>
       <c r="J17" s="31"/>
@@ -3415,16 +3430,16 @@
       <c r="D18" s="20"/>
       <c r="E18" s="82">
         <f>E17</f>
-        <v>44532</v>
+        <v>44531</v>
       </c>
       <c r="F18" s="82">
-        <f>E18+3</f>
-        <v>44535</v>
+        <f>E18+0</f>
+        <v>44531</v>
       </c>
       <c r="G18" s="14"/>
       <c r="H18" s="14">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I18" s="31"/>
       <c r="J18" s="31"/>
@@ -3559,17 +3574,17 @@
     <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="45"/>
       <c r="B20" s="64" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="C20" s="58"/>
       <c r="D20" s="23"/>
       <c r="E20" s="83">
-        <f>E9+15</f>
-        <v>44530</v>
+        <f>E9+16</f>
+        <v>44531</v>
       </c>
       <c r="F20" s="83">
         <f>E20+5</f>
-        <v>44535</v>
+        <v>44536</v>
       </c>
       <c r="G20" s="14"/>
       <c r="H20" s="14">
@@ -3636,22 +3651,22 @@
     <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="45"/>
       <c r="B21" s="64" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="C21" s="58"/>
       <c r="D21" s="23"/>
       <c r="E21" s="83">
         <f>F20+1</f>
-        <v>44536</v>
+        <v>44537</v>
       </c>
       <c r="F21" s="83">
-        <f>E21+4</f>
-        <v>44540</v>
+        <f>E21+8</f>
+        <v>44545</v>
       </c>
       <c r="G21" s="14"/>
       <c r="H21" s="14">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I21" s="31"/>
       <c r="J21" s="31"/>
@@ -3719,16 +3734,16 @@
       <c r="D22" s="23"/>
       <c r="E22" s="83">
         <f>E21+5</f>
-        <v>44541</v>
+        <v>44542</v>
       </c>
       <c r="F22" s="83">
-        <f>E22+5</f>
-        <v>44546</v>
+        <f>E22+0</f>
+        <v>44542</v>
       </c>
       <c r="G22" s="14"/>
       <c r="H22" s="14">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I22" s="31"/>
       <c r="J22" s="31"/>
@@ -3796,16 +3811,16 @@
       <c r="D23" s="23"/>
       <c r="E23" s="83">
         <f>F22+1</f>
-        <v>44547</v>
+        <v>44543</v>
       </c>
       <c r="F23" s="83">
-        <f>E23+4</f>
-        <v>44551</v>
+        <f>E23+0</f>
+        <v>44543</v>
       </c>
       <c r="G23" s="14"/>
       <c r="H23" s="14">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I23" s="31"/>
       <c r="J23" s="31"/>
@@ -3873,16 +3888,16 @@
       <c r="D24" s="23"/>
       <c r="E24" s="83">
         <f>E22</f>
-        <v>44541</v>
+        <v>44542</v>
       </c>
       <c r="F24" s="83">
-        <f>E24+4</f>
-        <v>44545</v>
+        <f>E24+0</f>
+        <v>44542</v>
       </c>
       <c r="G24" s="14"/>
       <c r="H24" s="14">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I24" s="31"/>
       <c r="J24" s="31"/>
@@ -4017,20 +4032,22 @@
     <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="45"/>
       <c r="B26" s="65" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="C26" s="60"/>
       <c r="D26" s="26"/>
-      <c r="E26" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="F26" s="84" t="s">
-        <v>26</v>
+      <c r="E26" s="84">
+        <f>F21</f>
+        <v>44545</v>
+      </c>
+      <c r="F26" s="84">
+        <f>E26+3</f>
+        <v>44548</v>
       </c>
       <c r="G26" s="14"/>
-      <c r="H26" s="14" t="e">
+      <c r="H26" s="14">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+        <v>4</v>
       </c>
       <c r="I26" s="31"/>
       <c r="J26" s="31"/>
@@ -4617,11 +4634,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -4629,6 +4641,11 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <conditionalFormatting sqref="D37:D38 D7:D30">
     <cfRule type="dataBar" priority="15">
@@ -4687,7 +4704,7 @@
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="F17 F21:F22 E22" formula="1"/>
+    <ignoredError sqref="E22" formula="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">

</xml_diff>